<commit_message>
[UI] DnD 및 새 빈 페이지 UI, 제스처 Dialog 추가 (#359)
* Design: 새 빈 페이지 생성 박스 색상 수정

* Design: DnD 시 표시 색상 수정

* Design: 제스처 첫 확인 시 알림 dialog 팝업
</commit_message>
<xml_diff>
--- a/src/GridaBoard/language/textData.xlsx
+++ b/src/GridaBoard/language/textData.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1450" uniqueCount="1094">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1458" uniqueCount="1102">
   <si>
     <t>Gridaboard 2.0 string</t>
   </si>
@@ -3198,6 +3198,31 @@
   </si>
   <si>
     <t>필기 숨기기</t>
+  </si>
+  <si>
+    <t>notice_gesture_title</t>
+  </si>
+  <si>
+    <t>스마트 제스처가 추가됐습니다!</t>
+  </si>
+  <si>
+    <t>notice_gesture_explain</t>
+  </si>
+  <si>
+    <t xml:space="preserve">지금 스마트 제스처 버튼을 누른 후, \n종이나 부기 보드에 스마트 제스처를 이용해보세요 !
+</t>
+  </si>
+  <si>
+    <t>notice_gesture_cancel</t>
+  </si>
+  <si>
+    <t>넘어가기</t>
+  </si>
+  <si>
+    <t>notice_gesture_success</t>
+  </si>
+  <si>
+    <t>더 알아보기</t>
   </si>
   <si>
     <t>title</t>
@@ -14105,10 +14130,14 @@
     <row r="237">
       <c r="A237" s="43"/>
       <c r="B237" s="116"/>
-      <c r="C237" s="114"/>
+      <c r="C237" s="200" t="s">
+        <v>1055</v>
+      </c>
       <c r="D237" s="113"/>
       <c r="E237" s="114"/>
-      <c r="F237" s="204"/>
+      <c r="F237" s="201" t="s">
+        <v>1056</v>
+      </c>
       <c r="G237" s="197"/>
       <c r="H237" s="197"/>
       <c r="I237" s="197"/>
@@ -14133,10 +14162,14 @@
     <row r="238">
       <c r="A238" s="43"/>
       <c r="B238" s="116"/>
-      <c r="C238" s="114"/>
+      <c r="C238" s="200" t="s">
+        <v>1057</v>
+      </c>
       <c r="D238" s="113"/>
       <c r="E238" s="114"/>
-      <c r="F238" s="204"/>
+      <c r="F238" s="201" t="s">
+        <v>1058</v>
+      </c>
       <c r="G238" s="197"/>
       <c r="H238" s="197"/>
       <c r="I238" s="197"/>
@@ -14161,10 +14194,14 @@
     <row r="239">
       <c r="A239" s="43"/>
       <c r="B239" s="116"/>
-      <c r="C239" s="114"/>
+      <c r="C239" s="200" t="s">
+        <v>1059</v>
+      </c>
       <c r="D239" s="113"/>
       <c r="E239" s="114"/>
-      <c r="F239" s="204"/>
+      <c r="F239" s="201" t="s">
+        <v>1060</v>
+      </c>
       <c r="G239" s="197"/>
       <c r="H239" s="197"/>
       <c r="I239" s="197"/>
@@ -14189,10 +14226,14 @@
     <row r="240">
       <c r="A240" s="43"/>
       <c r="B240" s="116"/>
-      <c r="C240" s="114"/>
+      <c r="C240" s="200" t="s">
+        <v>1061</v>
+      </c>
       <c r="D240" s="113"/>
       <c r="E240" s="114"/>
-      <c r="F240" s="204"/>
+      <c r="F240" s="201" t="s">
+        <v>1062</v>
+      </c>
       <c r="G240" s="197"/>
       <c r="H240" s="197"/>
       <c r="I240" s="197"/>
@@ -37119,22 +37160,22 @@
         <v>14</v>
       </c>
       <c r="B1" s="206" t="s">
-        <v>1055</v>
+        <v>1063</v>
       </c>
       <c r="C1" s="206" t="s">
-        <v>1056</v>
+        <v>1064</v>
       </c>
       <c r="D1" s="206" t="s">
-        <v>1057</v>
+        <v>1065</v>
       </c>
       <c r="E1" s="206" t="s">
-        <v>1058</v>
+        <v>1066</v>
       </c>
       <c r="F1" s="206" t="s">
-        <v>1059</v>
+        <v>1067</v>
       </c>
       <c r="G1" s="207" t="s">
-        <v>1060</v>
+        <v>1068</v>
       </c>
       <c r="H1" s="208"/>
       <c r="I1" s="208"/>
@@ -37158,21 +37199,21 @@
     </row>
     <row r="2">
       <c r="A2" s="208" t="s">
-        <v>1061</v>
+        <v>1069</v>
       </c>
       <c r="B2" s="208"/>
       <c r="C2" s="208"/>
       <c r="D2" s="175" t="s">
-        <v>1062</v>
+        <v>1070</v>
       </c>
       <c r="E2" s="209" t="s">
-        <v>1063</v>
+        <v>1071</v>
       </c>
       <c r="F2" s="210" t="s">
-        <v>1064</v>
+        <v>1072</v>
       </c>
       <c r="G2" s="211" t="s">
-        <v>1065</v>
+        <v>1073</v>
       </c>
       <c r="H2" s="208"/>
       <c r="I2" s="208"/>
@@ -37200,10 +37241,10 @@
       <c r="C3" s="208"/>
       <c r="D3" s="208"/>
       <c r="E3" s="209" t="s">
-        <v>1066</v>
+        <v>1074</v>
       </c>
       <c r="F3" s="212" t="s">
-        <v>1067</v>
+        <v>1075</v>
       </c>
       <c r="G3" s="213"/>
       <c r="H3" s="208"/>
@@ -37232,10 +37273,10 @@
       <c r="C4" s="208"/>
       <c r="D4" s="208"/>
       <c r="E4" s="209" t="s">
-        <v>1066</v>
+        <v>1074</v>
       </c>
       <c r="F4" s="212" t="s">
-        <v>1068</v>
+        <v>1076</v>
       </c>
       <c r="G4" s="213"/>
       <c r="H4" s="208"/>
@@ -37264,10 +37305,10 @@
       <c r="C5" s="208"/>
       <c r="D5" s="208"/>
       <c r="E5" s="209" t="s">
-        <v>1066</v>
+        <v>1074</v>
       </c>
       <c r="F5" s="214" t="s">
-        <v>1069</v>
+        <v>1077</v>
       </c>
       <c r="H5" s="208"/>
       <c r="I5" s="208"/>
@@ -37295,10 +37336,10 @@
       <c r="C6" s="208"/>
       <c r="D6" s="208"/>
       <c r="E6" s="209" t="s">
-        <v>1070</v>
+        <v>1078</v>
       </c>
       <c r="F6" s="214" t="s">
-        <v>1071</v>
+        <v>1079</v>
       </c>
       <c r="G6" s="215"/>
       <c r="H6" s="208"/>
@@ -37327,10 +37368,10 @@
       <c r="C7" s="208"/>
       <c r="D7" s="208"/>
       <c r="E7" s="216" t="s">
-        <v>1070</v>
+        <v>1078</v>
       </c>
       <c r="F7" s="217" t="s">
-        <v>1072</v>
+        <v>1080</v>
       </c>
       <c r="G7" s="215"/>
       <c r="H7" s="208"/>
@@ -37359,10 +37400,10 @@
       <c r="C8" s="208"/>
       <c r="D8" s="208"/>
       <c r="E8" s="218" t="s">
-        <v>1073</v>
+        <v>1081</v>
       </c>
       <c r="F8" s="218" t="s">
-        <v>1074</v>
+        <v>1082</v>
       </c>
       <c r="G8" s="146"/>
       <c r="H8" s="208"/>
@@ -37391,10 +37432,10 @@
       <c r="C9" s="208"/>
       <c r="D9" s="208"/>
       <c r="E9" s="218" t="s">
-        <v>1075</v>
+        <v>1083</v>
       </c>
       <c r="F9" s="218" t="s">
-        <v>1076</v>
+        <v>1084</v>
       </c>
       <c r="G9" s="219"/>
       <c r="H9" s="208"/>
@@ -37426,7 +37467,7 @@
         <v>515</v>
       </c>
       <c r="F10" s="221" t="s">
-        <v>1077</v>
+        <v>1085</v>
       </c>
       <c r="G10" s="219"/>
       <c r="H10" s="208"/>
@@ -37458,7 +37499,7 @@
         <v>515</v>
       </c>
       <c r="F11" s="218" t="s">
-        <v>1078</v>
+        <v>1086</v>
       </c>
       <c r="G11" s="146"/>
       <c r="H11" s="208"/>
@@ -37490,7 +37531,7 @@
         <v>515</v>
       </c>
       <c r="F12" s="222" t="s">
-        <v>1079</v>
+        <v>1087</v>
       </c>
       <c r="G12" s="219"/>
       <c r="H12" s="208"/>
@@ -37519,10 +37560,10 @@
       <c r="C13" s="208"/>
       <c r="D13" s="208"/>
       <c r="E13" s="218" t="s">
-        <v>1080</v>
+        <v>1088</v>
       </c>
       <c r="F13" s="218" t="s">
-        <v>1081</v>
+        <v>1089</v>
       </c>
       <c r="G13" s="146"/>
       <c r="H13" s="208"/>
@@ -37551,10 +37592,10 @@
       <c r="C14" s="208"/>
       <c r="D14" s="208"/>
       <c r="E14" s="218" t="s">
-        <v>1080</v>
+        <v>1088</v>
       </c>
       <c r="F14" s="218" t="s">
-        <v>1082</v>
+        <v>1090</v>
       </c>
       <c r="G14" s="146"/>
       <c r="H14" s="208"/>
@@ -37586,7 +37627,7 @@
         <v>18</v>
       </c>
       <c r="F15" s="218" t="s">
-        <v>1083</v>
+        <v>1091</v>
       </c>
       <c r="G15" s="146"/>
       <c r="H15" s="208"/>
@@ -37618,7 +37659,7 @@
         <v>18</v>
       </c>
       <c r="F16" s="218" t="s">
-        <v>1084</v>
+        <v>1092</v>
       </c>
       <c r="G16" s="146"/>
       <c r="H16" s="208"/>
@@ -37650,7 +37691,7 @@
         <v>18</v>
       </c>
       <c r="F17" s="218" t="s">
-        <v>1085</v>
+        <v>1093</v>
       </c>
       <c r="G17" s="146"/>
       <c r="H17" s="208"/>
@@ -37679,10 +37720,10 @@
       <c r="C18" s="208"/>
       <c r="D18" s="208"/>
       <c r="E18" s="223" t="s">
-        <v>1086</v>
+        <v>1094</v>
       </c>
       <c r="F18" s="218" t="s">
-        <v>1087</v>
+        <v>1095</v>
       </c>
       <c r="G18" s="146"/>
       <c r="H18" s="208"/>
@@ -37735,18 +37776,18 @@
     </row>
     <row r="20">
       <c r="A20" s="211" t="s">
-        <v>1088</v>
+        <v>1096</v>
       </c>
       <c r="B20" s="208"/>
       <c r="C20" s="208"/>
       <c r="D20" s="211" t="s">
-        <v>1062</v>
+        <v>1070</v>
       </c>
       <c r="E20" s="211" t="s">
-        <v>1089</v>
+        <v>1097</v>
       </c>
       <c r="F20" s="219" t="s">
-        <v>1090</v>
+        <v>1098</v>
       </c>
       <c r="G20" s="146"/>
       <c r="H20" s="208"/>
@@ -37775,10 +37816,10 @@
       <c r="C21" s="208"/>
       <c r="D21" s="208"/>
       <c r="E21" s="211" t="s">
-        <v>1091</v>
+        <v>1099</v>
       </c>
       <c r="F21" s="219" t="s">
-        <v>1092</v>
+        <v>1100</v>
       </c>
       <c r="G21" s="219"/>
       <c r="H21" s="208"/>
@@ -37807,10 +37848,10 @@
       <c r="C22" s="208"/>
       <c r="D22" s="208"/>
       <c r="E22" s="211" t="s">
-        <v>1091</v>
+        <v>1099</v>
       </c>
       <c r="F22" s="226" t="s">
-        <v>1093</v>
+        <v>1101</v>
       </c>
       <c r="G22" s="219"/>
       <c r="H22" s="208"/>

</xml_diff>

<commit_message>
Fix: 다국어 지원을 위한 plate/page mode text -> getText()로 불러오도록 수정
</commit_message>
<xml_diff>
--- a/src/GridaBoard/language/textData.xlsx
+++ b/src/GridaBoard/language/textData.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1474" uniqueCount="1118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1480" uniqueCount="1122">
   <si>
     <t>Gridaboard 2.0 string</t>
   </si>
@@ -3229,6 +3229,18 @@
   </si>
   <si>
     <t>읽을 수 없는 파일입니다. 파일명을 확인해주세요.</t>
+  </si>
+  <si>
+    <t>nav_plate_mode</t>
+  </si>
+  <si>
+    <t>PLATE MODE</t>
+  </si>
+  <si>
+    <t>nav_page_mode</t>
+  </si>
+  <si>
+    <t>PAGE MODE</t>
   </si>
   <si>
     <t>title</t>
@@ -14325,11 +14337,17 @@
     <row r="242">
       <c r="A242" s="43"/>
       <c r="B242" s="116"/>
-      <c r="C242" s="114"/>
+      <c r="C242" s="112" t="s">
+        <v>1065</v>
+      </c>
       <c r="D242" s="113"/>
       <c r="E242" s="114"/>
-      <c r="F242" s="201"/>
-      <c r="G242" s="197"/>
+      <c r="F242" s="170" t="s">
+        <v>1066</v>
+      </c>
+      <c r="G242" s="170" t="s">
+        <v>1066</v>
+      </c>
       <c r="H242" s="197"/>
       <c r="I242" s="197"/>
       <c r="J242" s="53"/>
@@ -14353,11 +14371,17 @@
     <row r="243">
       <c r="A243" s="43"/>
       <c r="B243" s="116"/>
-      <c r="C243" s="114"/>
+      <c r="C243" s="112" t="s">
+        <v>1067</v>
+      </c>
       <c r="D243" s="113"/>
       <c r="E243" s="114"/>
-      <c r="F243" s="201"/>
-      <c r="G243" s="197"/>
+      <c r="F243" s="170" t="s">
+        <v>1068</v>
+      </c>
+      <c r="G243" s="170" t="s">
+        <v>1068</v>
+      </c>
       <c r="H243" s="197"/>
       <c r="I243" s="197"/>
       <c r="J243" s="53"/>
@@ -37199,22 +37223,22 @@
         <v>14</v>
       </c>
       <c r="B1" s="203" t="s">
-        <v>1065</v>
+        <v>1069</v>
       </c>
       <c r="C1" s="203" t="s">
-        <v>1066</v>
+        <v>1070</v>
       </c>
       <c r="D1" s="203" t="s">
-        <v>1067</v>
+        <v>1071</v>
       </c>
       <c r="E1" s="203" t="s">
-        <v>1068</v>
+        <v>1072</v>
       </c>
       <c r="F1" s="203" t="s">
-        <v>1069</v>
+        <v>1073</v>
       </c>
       <c r="G1" s="204" t="s">
-        <v>1070</v>
+        <v>1074</v>
       </c>
       <c r="H1" s="205"/>
       <c r="I1" s="205"/>
@@ -37238,21 +37262,21 @@
     </row>
     <row r="2">
       <c r="A2" s="205" t="s">
-        <v>1071</v>
+        <v>1075</v>
       </c>
       <c r="B2" s="205"/>
       <c r="C2" s="205"/>
       <c r="D2" s="175" t="s">
-        <v>1072</v>
+        <v>1076</v>
       </c>
       <c r="E2" s="206" t="s">
-        <v>1073</v>
+        <v>1077</v>
       </c>
       <c r="F2" s="207" t="s">
-        <v>1074</v>
+        <v>1078</v>
       </c>
       <c r="G2" s="208" t="s">
-        <v>1075</v>
+        <v>1079</v>
       </c>
       <c r="H2" s="205"/>
       <c r="I2" s="205"/>
@@ -37280,10 +37304,10 @@
       <c r="C3" s="205"/>
       <c r="D3" s="205"/>
       <c r="E3" s="206" t="s">
-        <v>1076</v>
+        <v>1080</v>
       </c>
       <c r="F3" s="209" t="s">
-        <v>1077</v>
+        <v>1081</v>
       </c>
       <c r="G3" s="210"/>
       <c r="H3" s="205"/>
@@ -37312,10 +37336,10 @@
       <c r="C4" s="205"/>
       <c r="D4" s="205"/>
       <c r="E4" s="206" t="s">
-        <v>1076</v>
+        <v>1080</v>
       </c>
       <c r="F4" s="209" t="s">
-        <v>1078</v>
+        <v>1082</v>
       </c>
       <c r="G4" s="210"/>
       <c r="H4" s="205"/>
@@ -37344,10 +37368,10 @@
       <c r="C5" s="205"/>
       <c r="D5" s="205"/>
       <c r="E5" s="206" t="s">
-        <v>1076</v>
+        <v>1080</v>
       </c>
       <c r="F5" s="211" t="s">
-        <v>1079</v>
+        <v>1083</v>
       </c>
       <c r="H5" s="205"/>
       <c r="I5" s="205"/>
@@ -37375,10 +37399,10 @@
       <c r="C6" s="205"/>
       <c r="D6" s="205"/>
       <c r="E6" s="206" t="s">
-        <v>1080</v>
+        <v>1084</v>
       </c>
       <c r="F6" s="211" t="s">
-        <v>1081</v>
+        <v>1085</v>
       </c>
       <c r="G6" s="212"/>
       <c r="H6" s="205"/>
@@ -37407,10 +37431,10 @@
       <c r="C7" s="205"/>
       <c r="D7" s="205"/>
       <c r="E7" s="213" t="s">
-        <v>1080</v>
+        <v>1084</v>
       </c>
       <c r="F7" s="214" t="s">
-        <v>1082</v>
+        <v>1086</v>
       </c>
       <c r="G7" s="212"/>
       <c r="H7" s="205"/>
@@ -37439,10 +37463,10 @@
       <c r="C8" s="205"/>
       <c r="D8" s="205"/>
       <c r="E8" s="215" t="s">
-        <v>1083</v>
+        <v>1087</v>
       </c>
       <c r="F8" s="215" t="s">
-        <v>1084</v>
+        <v>1088</v>
       </c>
       <c r="G8" s="146"/>
       <c r="H8" s="205"/>
@@ -37471,10 +37495,10 @@
       <c r="C9" s="205"/>
       <c r="D9" s="205"/>
       <c r="E9" s="215" t="s">
-        <v>1085</v>
+        <v>1089</v>
       </c>
       <c r="F9" s="215" t="s">
-        <v>1086</v>
+        <v>1090</v>
       </c>
       <c r="G9" s="216"/>
       <c r="H9" s="205"/>
@@ -37506,7 +37530,7 @@
         <v>515</v>
       </c>
       <c r="F10" s="218" t="s">
-        <v>1087</v>
+        <v>1091</v>
       </c>
       <c r="G10" s="216"/>
       <c r="H10" s="205"/>
@@ -37538,7 +37562,7 @@
         <v>515</v>
       </c>
       <c r="F11" s="215" t="s">
-        <v>1088</v>
+        <v>1092</v>
       </c>
       <c r="G11" s="146"/>
       <c r="H11" s="205"/>
@@ -37570,7 +37594,7 @@
         <v>515</v>
       </c>
       <c r="F12" s="219" t="s">
-        <v>1089</v>
+        <v>1093</v>
       </c>
       <c r="G12" s="216"/>
       <c r="H12" s="205"/>
@@ -37599,10 +37623,10 @@
       <c r="C13" s="205"/>
       <c r="D13" s="205"/>
       <c r="E13" s="215" t="s">
-        <v>1090</v>
+        <v>1094</v>
       </c>
       <c r="F13" s="215" t="s">
-        <v>1091</v>
+        <v>1095</v>
       </c>
       <c r="G13" s="146"/>
       <c r="H13" s="205"/>
@@ -37631,10 +37655,10 @@
       <c r="C14" s="205"/>
       <c r="D14" s="205"/>
       <c r="E14" s="215" t="s">
-        <v>1090</v>
+        <v>1094</v>
       </c>
       <c r="F14" s="215" t="s">
-        <v>1092</v>
+        <v>1096</v>
       </c>
       <c r="G14" s="146"/>
       <c r="H14" s="205"/>
@@ -37666,7 +37690,7 @@
         <v>18</v>
       </c>
       <c r="F15" s="215" t="s">
-        <v>1093</v>
+        <v>1097</v>
       </c>
       <c r="G15" s="146"/>
       <c r="H15" s="205"/>
@@ -37698,7 +37722,7 @@
         <v>18</v>
       </c>
       <c r="F16" s="215" t="s">
-        <v>1094</v>
+        <v>1098</v>
       </c>
       <c r="G16" s="146"/>
       <c r="H16" s="205"/>
@@ -37730,7 +37754,7 @@
         <v>18</v>
       </c>
       <c r="F17" s="215" t="s">
-        <v>1095</v>
+        <v>1099</v>
       </c>
       <c r="G17" s="146"/>
       <c r="H17" s="205"/>
@@ -37759,10 +37783,10 @@
       <c r="C18" s="205"/>
       <c r="D18" s="205"/>
       <c r="E18" s="220" t="s">
-        <v>1096</v>
+        <v>1100</v>
       </c>
       <c r="F18" s="215" t="s">
-        <v>1097</v>
+        <v>1101</v>
       </c>
       <c r="G18" s="146"/>
       <c r="H18" s="205"/>
@@ -37815,18 +37839,18 @@
     </row>
     <row r="20">
       <c r="A20" s="208" t="s">
-        <v>1098</v>
+        <v>1102</v>
       </c>
       <c r="B20" s="205"/>
       <c r="C20" s="205"/>
       <c r="D20" s="208" t="s">
-        <v>1072</v>
+        <v>1076</v>
       </c>
       <c r="E20" s="208" t="s">
-        <v>1099</v>
+        <v>1103</v>
       </c>
       <c r="F20" s="216" t="s">
-        <v>1100</v>
+        <v>1104</v>
       </c>
       <c r="G20" s="146"/>
       <c r="H20" s="205"/>
@@ -37855,10 +37879,10 @@
       <c r="C21" s="205"/>
       <c r="D21" s="205"/>
       <c r="E21" s="208" t="s">
-        <v>1101</v>
+        <v>1105</v>
       </c>
       <c r="F21" s="216" t="s">
-        <v>1102</v>
+        <v>1106</v>
       </c>
       <c r="G21" s="216"/>
       <c r="H21" s="205"/>
@@ -37887,10 +37911,10 @@
       <c r="C22" s="205"/>
       <c r="D22" s="205"/>
       <c r="E22" s="208" t="s">
-        <v>1101</v>
+        <v>1105</v>
       </c>
       <c r="F22" s="223" t="s">
-        <v>1103</v>
+        <v>1107</v>
       </c>
       <c r="G22" s="216"/>
       <c r="H22" s="205"/>
@@ -37943,18 +37967,18 @@
     </row>
     <row r="24">
       <c r="A24" s="224" t="s">
-        <v>1104</v>
+        <v>1108</v>
       </c>
       <c r="B24" s="205"/>
       <c r="C24" s="205"/>
       <c r="D24" s="224" t="s">
-        <v>1105</v>
+        <v>1109</v>
       </c>
       <c r="E24" s="175" t="s">
-        <v>1106</v>
+        <v>1110</v>
       </c>
       <c r="F24" s="175" t="s">
-        <v>1107</v>
+        <v>1111</v>
       </c>
       <c r="G24" s="225"/>
       <c r="H24" s="205"/>
@@ -37983,10 +38007,10 @@
       <c r="C25" s="205"/>
       <c r="D25" s="205"/>
       <c r="E25" s="175" t="s">
-        <v>1108</v>
+        <v>1112</v>
       </c>
       <c r="F25" s="175" t="s">
-        <v>1109</v>
+        <v>1113</v>
       </c>
       <c r="G25" s="146"/>
       <c r="H25" s="205"/>
@@ -38015,10 +38039,10 @@
       <c r="C26" s="205"/>
       <c r="D26" s="205"/>
       <c r="E26" s="175" t="s">
-        <v>1110</v>
+        <v>1114</v>
       </c>
       <c r="F26" s="175" t="s">
-        <v>1111</v>
+        <v>1115</v>
       </c>
       <c r="G26" s="146"/>
       <c r="H26" s="205"/>
@@ -38047,10 +38071,10 @@
       <c r="C27" s="205"/>
       <c r="D27" s="205"/>
       <c r="E27" s="175" t="s">
-        <v>1112</v>
+        <v>1116</v>
       </c>
       <c r="F27" s="175" t="s">
-        <v>1113</v>
+        <v>1117</v>
       </c>
       <c r="G27" s="146"/>
       <c r="H27" s="205"/>
@@ -38079,10 +38103,10 @@
       <c r="C28" s="205"/>
       <c r="D28" s="205"/>
       <c r="E28" s="175" t="s">
-        <v>1114</v>
+        <v>1118</v>
       </c>
       <c r="F28" s="175" t="s">
-        <v>1115</v>
+        <v>1119</v>
       </c>
       <c r="G28" s="146"/>
       <c r="H28" s="205"/>
@@ -38111,10 +38135,10 @@
       <c r="C29" s="205"/>
       <c r="D29" s="205"/>
       <c r="E29" s="224" t="s">
-        <v>1116</v>
+        <v>1120</v>
       </c>
       <c r="F29" s="226" t="s">
-        <v>1117</v>
+        <v>1121</v>
       </c>
       <c r="G29" s="146"/>
       <c r="H29" s="205"/>

</xml_diff>